<commit_message>
5.3-main- Updated INS results on the Excel file with results.
</commit_message>
<xml_diff>
--- a/Navigation Solutions/Results_main_file.xlsx
+++ b/Navigation Solutions/Results_main_file.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eudald\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eudald\Documents\Git Repos\Effect-of-Adding-Time-Correlation-to-SVM-based-Motion-Classification-in-Pedestrian-Navigation\Navigation Solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02BF10B-EA1F-4674-866F-B3498489CCE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F37454-3F09-4187-AE13-8EAFFE45E452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{62F6A1EA-9600-4F06-81D9-19BA584D623D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
   <si>
     <t>exp100</t>
   </si>
@@ -110,12 +110,6 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>Improvement Time Series vs standard SVM</t>
-  </si>
-  <si>
-    <t>Improvement Time Series vs SHOE</t>
-  </si>
-  <si>
     <t>exp1200</t>
   </si>
   <si>
@@ -127,7 +121,37 @@
   </si>
   <si>
     <t>Thresholds per each
- subject</t>
+ activity across subjects</t>
+  </si>
+  <si>
+    <t>Fixed Threshold</t>
+  </si>
+  <si>
+    <t>Thresholdless</t>
+  </si>
+  <si>
+    <t>Pure INS</t>
+  </si>
+  <si>
+    <t>INS</t>
+  </si>
+  <si>
+    <t>ZUPT-SVM  (TS SVM) vs standard SVM</t>
+  </si>
+  <si>
+    <t>ZUPT-SVM  (TS SVM) vs SHOE</t>
+  </si>
+  <si>
+    <t>ZUPT-SVM  (TS SVM) vs INS</t>
+  </si>
+  <si>
+    <t>ZUPT-SVM-SHOE (TS SVM) vs standard SVM</t>
+  </si>
+  <si>
+    <t>ZUPT-SVM-SHOE (TS SVM) vs SHOE</t>
+  </si>
+  <si>
+    <t>ZUPT-SVM-SHOE (TS SVM) vs INS</t>
   </si>
 </sst>
 </file>
@@ -157,7 +181,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,6 +197,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -306,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -338,24 +380,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -374,6 +398,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,74 +760,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5063AEB1-AEEA-4805-8B48-BD54CBCBC4C5}">
-  <dimension ref="B2:Q45"/>
+  <dimension ref="B2:S48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5:M5"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.42578125" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" customWidth="1"/>
-    <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" customWidth="1"/>
+    <col min="18" max="18" width="11" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="29" t="s">
+    <row r="2" spans="2:19" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="37"/>
+      <c r="F2" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="27" t="s">
+      <c r="G2" s="36"/>
+      <c r="H2" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-    </row>
-    <row r="3" spans="2:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="34" t="s">
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+    </row>
+    <row r="3" spans="2:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="29"/>
+      <c r="F3" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="23" t="s">
+      <c r="G3" s="29"/>
+      <c r="H3" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25" t="s">
+      <c r="I3" s="31"/>
+      <c r="J3" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="23" t="s">
+      <c r="K3" s="29"/>
+      <c r="L3" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="24"/>
-      <c r="L3" s="25" t="s">
+      <c r="M3" s="31"/>
+      <c r="N3" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="26"/>
-      <c r="N3" s="23" t="s">
+      <c r="O3" s="29"/>
+      <c r="P3" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="24"/>
-      <c r="P3" s="25" t="s">
+      <c r="Q3" s="31"/>
+      <c r="R3" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="26"/>
-    </row>
-    <row r="4" spans="2:17" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S3" s="29"/>
+    </row>
+    <row r="4" spans="2:19" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="4" t="s">
         <v>13</v>
       </c>
@@ -785,1644 +857,1846 @@
       <c r="F4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="P4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
+      <c r="R4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="25" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="2">
+        <v>75.309399999999997</v>
+      </c>
+      <c r="E5" s="2">
+        <v>345.12310000000002</v>
+      </c>
+      <c r="F5" s="7">
         <v>4.6974</v>
       </c>
-      <c r="E5" s="8">
+      <c r="G5" s="8">
         <v>1.4516</v>
       </c>
-      <c r="F5" s="7">
+      <c r="H5" s="7">
         <v>3.8826000000000001</v>
       </c>
-      <c r="G5" s="9">
+      <c r="I5" s="9">
         <v>1.4595</v>
       </c>
-      <c r="H5" s="9">
+      <c r="J5" s="9">
         <v>3.371</v>
       </c>
-      <c r="I5" s="8">
+      <c r="K5" s="8">
         <v>1.7070000000000001</v>
       </c>
-      <c r="J5" s="7">
+      <c r="L5" s="7">
         <v>3.8639000000000001</v>
       </c>
-      <c r="K5" s="9">
+      <c r="M5" s="9">
         <v>1.1913</v>
       </c>
-      <c r="L5" s="9">
+      <c r="N5" s="9">
         <v>3.3409</v>
       </c>
-      <c r="M5" s="8">
+      <c r="O5" s="8">
         <v>1.3788</v>
       </c>
-      <c r="N5" s="7">
+      <c r="P5" s="7">
         <v>4.8554000000000004</v>
       </c>
-      <c r="O5" s="9">
+      <c r="Q5" s="9">
         <v>0.97119999999999995</v>
       </c>
-      <c r="P5" s="9">
+      <c r="R5" s="9">
         <v>4.17</v>
       </c>
-      <c r="Q5" s="8">
+      <c r="S5" s="8">
         <v>2.8283999999999998</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="32"/>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="26"/>
       <c r="C6" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6">
+        <v>215.33580000000001</v>
+      </c>
+      <c r="E6">
+        <v>898.24659999999994</v>
+      </c>
+      <c r="F6" s="10">
         <v>65.912599999999998</v>
       </c>
-      <c r="E6" s="11">
+      <c r="G6" s="11">
         <v>71.017399999999995</v>
       </c>
-      <c r="F6" s="10">
+      <c r="H6" s="10">
         <v>14.067</v>
       </c>
-      <c r="G6" s="12">
+      <c r="I6" s="12">
         <v>14.5328</v>
       </c>
-      <c r="H6" s="12">
+      <c r="J6" s="12">
         <v>14.035</v>
       </c>
-      <c r="I6" s="11">
+      <c r="K6" s="11">
         <v>12.965299999999999</v>
       </c>
-      <c r="J6" s="10">
+      <c r="L6" s="10">
         <v>13.9648</v>
       </c>
-      <c r="K6" s="12">
+      <c r="M6" s="12">
         <v>12.592599999999999</v>
       </c>
-      <c r="L6" s="12">
+      <c r="N6" s="12">
         <v>13.4419</v>
       </c>
-      <c r="M6" s="11">
+      <c r="O6" s="11">
         <v>11.758699999999999</v>
       </c>
-      <c r="N6" s="10">
+      <c r="P6" s="10">
         <v>12.885400000000001</v>
       </c>
-      <c r="O6" s="12">
+      <c r="Q6" s="12">
         <v>11.604100000000001</v>
       </c>
-      <c r="P6" s="12">
+      <c r="R6" s="12">
         <v>12.7507</v>
       </c>
-      <c r="Q6" s="11">
+      <c r="S6" s="11">
         <v>12.612399999999999</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="32"/>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="26"/>
       <c r="C7" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7">
+        <v>218.846</v>
+      </c>
+      <c r="E7">
+        <v>839.34789999999998</v>
+      </c>
+      <c r="F7" s="10">
         <v>56.8568</v>
       </c>
-      <c r="E7" s="11">
+      <c r="G7" s="11">
         <v>69.319500000000005</v>
       </c>
-      <c r="F7" s="10">
+      <c r="H7" s="10">
         <v>6.4660000000000002</v>
       </c>
-      <c r="G7" s="12">
+      <c r="I7" s="12">
         <v>12.333399999999999</v>
       </c>
-      <c r="H7" s="12">
+      <c r="J7" s="12">
         <v>6.0507999999999997</v>
       </c>
-      <c r="I7" s="11">
+      <c r="K7" s="11">
         <v>10.1959</v>
       </c>
-      <c r="J7" s="10">
+      <c r="L7" s="10">
         <v>6.6102999999999996</v>
       </c>
-      <c r="K7" s="12">
+      <c r="M7" s="12">
         <v>10.588100000000001</v>
       </c>
-      <c r="L7" s="12">
+      <c r="N7" s="12">
         <v>5.4036999999999997</v>
       </c>
-      <c r="M7" s="11">
+      <c r="O7" s="11">
         <v>9.1597000000000008</v>
       </c>
-      <c r="N7" s="10">
+      <c r="P7" s="10">
         <v>6.7892000000000001</v>
       </c>
-      <c r="O7" s="12">
+      <c r="Q7" s="12">
         <v>10.2841</v>
       </c>
-      <c r="P7" s="12">
+      <c r="R7" s="12">
         <v>7.6588000000000003</v>
       </c>
-      <c r="Q7" s="11">
+      <c r="S7" s="11">
         <v>9.5630000000000006</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="32"/>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="26"/>
       <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
       <c r="F8" s="10"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="11"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="32"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="11"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="26"/>
       <c r="C9" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9">
+        <v>274.29599999999999</v>
+      </c>
+      <c r="E9">
+        <v>432.11270000000002</v>
+      </c>
+      <c r="F9" s="10">
         <v>7.3547000000000002</v>
       </c>
-      <c r="E9" s="11">
+      <c r="G9" s="11">
         <v>10.34</v>
       </c>
-      <c r="F9" s="10">
+      <c r="H9" s="10">
         <v>5.0492999999999997</v>
       </c>
-      <c r="G9" s="12">
+      <c r="I9" s="12">
         <v>4.1772999999999998</v>
       </c>
-      <c r="H9" s="12">
+      <c r="J9" s="12">
         <v>6.0507999999999997</v>
       </c>
-      <c r="I9" s="11">
+      <c r="K9" s="11">
         <v>10.1959</v>
       </c>
-      <c r="J9" s="10">
+      <c r="L9" s="10">
         <v>4.9858000000000002</v>
       </c>
-      <c r="K9" s="12">
+      <c r="M9" s="12">
         <v>1.8166</v>
       </c>
-      <c r="L9" s="12">
+      <c r="N9" s="12">
         <v>5.6268000000000002</v>
       </c>
-      <c r="M9" s="11">
+      <c r="O9" s="11">
         <v>2.1267</v>
       </c>
-      <c r="N9" s="10">
+      <c r="P9" s="10">
         <v>5.1115000000000004</v>
       </c>
-      <c r="O9" s="12">
+      <c r="Q9" s="12">
         <v>1.8909</v>
       </c>
-      <c r="P9" s="12">
+      <c r="R9" s="12">
         <v>5.4504999999999999</v>
       </c>
-      <c r="Q9" s="11">
+      <c r="S9" s="11">
         <v>2.8348</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="32"/>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B10" s="26"/>
       <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10">
+        <v>4739.9192000000003</v>
+      </c>
+      <c r="E10">
+        <v>1920.4458999999999</v>
+      </c>
+      <c r="F10" s="10">
         <v>19.041499999999999</v>
       </c>
-      <c r="E10" s="11">
+      <c r="G10" s="11">
         <v>23.017399999999999</v>
       </c>
-      <c r="F10" s="10">
+      <c r="H10" s="10">
         <v>6.4307999999999996</v>
       </c>
-      <c r="G10" s="12">
+      <c r="I10" s="12">
         <v>5.2384000000000004</v>
       </c>
-      <c r="H10" s="12">
+      <c r="J10" s="12">
         <v>2.7467999999999999</v>
       </c>
-      <c r="I10" s="11">
+      <c r="K10" s="11">
         <v>4.1132</v>
       </c>
-      <c r="J10" s="10">
+      <c r="L10" s="10">
         <v>6.6425000000000001</v>
       </c>
-      <c r="K10" s="12">
+      <c r="M10" s="12">
         <v>5.2746000000000004</v>
       </c>
-      <c r="L10" s="12">
+      <c r="N10" s="12">
         <v>2.8969999999999998</v>
       </c>
-      <c r="M10" s="11">
+      <c r="O10" s="11">
         <v>4.8548</v>
       </c>
-      <c r="N10" s="10">
+      <c r="P10" s="10">
         <v>6.9455</v>
       </c>
-      <c r="O10" s="12">
+      <c r="Q10" s="12">
         <v>4.4321999999999999</v>
       </c>
-      <c r="P10" s="12">
+      <c r="R10" s="12">
         <v>7.8013000000000003</v>
       </c>
-      <c r="Q10" s="11">
+      <c r="S10" s="11">
         <v>6.0419999999999998</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="32"/>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B11" s="26"/>
       <c r="C11" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11">
+        <v>1876.6866</v>
+      </c>
+      <c r="E11">
+        <v>1322.2140999999999</v>
+      </c>
+      <c r="F11" s="10">
         <v>8.9520999999999997</v>
       </c>
-      <c r="E11" s="11">
+      <c r="G11" s="11">
         <v>14.395899999999999</v>
       </c>
-      <c r="F11" s="10">
+      <c r="H11" s="10">
         <v>1.6431</v>
       </c>
-      <c r="G11" s="12">
+      <c r="I11" s="12">
         <v>2.3321999999999998</v>
       </c>
-      <c r="H11" s="12">
+      <c r="J11" s="12">
         <v>2.2890000000000001</v>
       </c>
-      <c r="I11" s="11">
+      <c r="K11" s="11">
         <v>2.0142000000000002</v>
       </c>
-      <c r="J11" s="10">
+      <c r="L11" s="10">
         <v>2.5160999999999998</v>
       </c>
-      <c r="K11" s="12">
+      <c r="M11" s="12">
         <v>2.4422000000000001</v>
       </c>
-      <c r="L11" s="12">
+      <c r="N11" s="12">
         <v>2.4773999999999998</v>
       </c>
-      <c r="M11" s="11">
+      <c r="O11" s="11">
         <v>2.1798999999999999</v>
       </c>
-      <c r="N11" s="10">
+      <c r="P11" s="10">
         <v>6.101</v>
       </c>
-      <c r="O11" s="12">
+      <c r="Q11" s="12">
         <v>2.7505999999999999</v>
       </c>
-      <c r="P11" s="12">
+      <c r="R11" s="12">
         <v>11.0474</v>
       </c>
-      <c r="Q11" s="11">
+      <c r="S11" s="11">
         <v>3.4540000000000002</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="32"/>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="26"/>
       <c r="C12" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12">
+        <v>667.65679999999998</v>
+      </c>
+      <c r="E12">
+        <v>1764.3495</v>
+      </c>
+      <c r="F12" s="10">
         <v>30.649899999999999</v>
       </c>
-      <c r="E12" s="11">
+      <c r="G12" s="11">
         <v>37.227899999999998</v>
       </c>
-      <c r="F12" s="10">
+      <c r="H12" s="10">
         <v>6.5632000000000001</v>
       </c>
-      <c r="G12" s="12">
+      <c r="I12" s="12">
         <v>8.0717999999999996</v>
       </c>
-      <c r="H12" s="12">
+      <c r="J12" s="12">
         <v>5.3132000000000001</v>
       </c>
-      <c r="I12" s="11">
+      <c r="K12" s="11">
         <v>6.0019999999999998</v>
       </c>
-      <c r="J12" s="10">
+      <c r="L12" s="10">
         <v>9.1712000000000007</v>
       </c>
-      <c r="K12" s="12">
+      <c r="M12" s="12">
         <v>7.3030999999999997</v>
       </c>
-      <c r="L12" s="12">
+      <c r="N12" s="12">
         <v>7.1928000000000001</v>
       </c>
-      <c r="M12" s="11">
+      <c r="O12" s="11">
         <v>7.8551000000000002</v>
       </c>
-      <c r="N12" s="10">
+      <c r="P12" s="10">
         <v>10.3858</v>
       </c>
-      <c r="O12" s="12">
+      <c r="Q12" s="12">
         <v>7.4875999999999996</v>
       </c>
-      <c r="P12" s="12">
+      <c r="R12" s="12">
         <v>13.1587</v>
       </c>
-      <c r="Q12" s="11">
+      <c r="S12" s="11">
         <v>8.8741000000000003</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="32"/>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="26"/>
       <c r="C13" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13">
+        <v>2297.7159999999999</v>
+      </c>
+      <c r="E13">
+        <v>1657.1914999999999</v>
+      </c>
+      <c r="F13" s="10">
         <v>17.467600000000001</v>
       </c>
-      <c r="E13" s="11">
+      <c r="G13" s="11">
         <v>22.3782</v>
       </c>
-      <c r="F13" s="10">
+      <c r="H13" s="10">
         <v>2.4028999999999998</v>
       </c>
-      <c r="G13" s="12">
+      <c r="I13" s="12">
         <v>3.0097999999999998</v>
       </c>
-      <c r="H13" s="12">
+      <c r="J13" s="12">
         <v>6.3320999999999996</v>
       </c>
-      <c r="I13" s="11">
+      <c r="K13" s="11">
         <v>3.1812</v>
       </c>
-      <c r="J13" s="10">
+      <c r="L13" s="10">
         <v>3.7505000000000002</v>
       </c>
-      <c r="K13" s="12">
+      <c r="M13" s="12">
         <v>3.8437999999999999</v>
       </c>
-      <c r="L13" s="12">
+      <c r="N13" s="12">
         <v>5.9932999999999996</v>
       </c>
-      <c r="M13" s="11">
+      <c r="O13" s="11">
         <v>4.1814</v>
       </c>
-      <c r="N13" s="10">
+      <c r="P13" s="10">
         <v>6.0650000000000004</v>
       </c>
-      <c r="O13" s="12">
+      <c r="Q13" s="12">
         <v>4.0426000000000002</v>
       </c>
-      <c r="P13" s="12">
+      <c r="R13" s="12">
         <v>17.1157</v>
       </c>
-      <c r="Q13" s="11">
+      <c r="S13" s="11">
         <v>5.9111000000000002</v>
       </c>
     </row>
-    <row r="14" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="33"/>
+    <row r="14" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="27"/>
       <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="1">
+        <v>264.64400000000001</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1251.0477000000001</v>
+      </c>
+      <c r="F14" s="13">
         <v>36.534300000000002</v>
       </c>
-      <c r="E14" s="14">
+      <c r="G14" s="14">
         <v>37.369900000000001</v>
       </c>
-      <c r="F14" s="13">
+      <c r="H14" s="13">
         <v>6.5632000000000001</v>
       </c>
-      <c r="G14" s="15">
+      <c r="I14" s="15">
         <v>8.0717999999999996</v>
       </c>
-      <c r="H14" s="15">
+      <c r="J14" s="15">
         <v>5.4775</v>
       </c>
-      <c r="I14" s="14">
+      <c r="K14" s="14">
         <v>6.9004000000000003</v>
       </c>
-      <c r="J14" s="13">
+      <c r="L14" s="13">
         <v>7.6578999999999997</v>
       </c>
-      <c r="K14" s="15">
+      <c r="M14" s="15">
         <v>7.0641999999999996</v>
       </c>
-      <c r="L14" s="15">
+      <c r="N14" s="15">
         <v>5.9882</v>
       </c>
-      <c r="M14" s="14">
+      <c r="O14" s="14">
         <v>6.4790999999999999</v>
       </c>
-      <c r="N14" s="13">
+      <c r="P14" s="13">
         <v>9.0139999999999993</v>
       </c>
-      <c r="O14" s="15">
+      <c r="Q14" s="15">
         <v>6.9737999999999998</v>
       </c>
-      <c r="P14" s="15">
+      <c r="R14" s="15">
         <v>12.0595</v>
       </c>
-      <c r="Q14" s="14">
+      <c r="S14" s="14">
         <v>7.8365999999999998</v>
       </c>
     </row>
-    <row r="15" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="16">
-        <f t="shared" ref="D15:Q15" si="0">SUM(D5:D14)/9</f>
-        <v>27.496322222222222</v>
+        <f t="shared" ref="D15:S15" si="0">SUM(D5:D14)/9</f>
+        <v>1181.1566444444443</v>
       </c>
       <c r="E15" s="17">
         <f t="shared" si="0"/>
-        <v>31.835311111111114</v>
+        <v>1158.8976666666667</v>
       </c>
       <c r="F15" s="16">
         <f t="shared" si="0"/>
-        <v>5.8964555555555558</v>
+        <v>27.496322222222222</v>
       </c>
       <c r="G15" s="17">
         <f t="shared" si="0"/>
+        <v>31.835311111111114</v>
+      </c>
+      <c r="H15" s="16">
+        <f t="shared" si="0"/>
+        <v>5.8964555555555558</v>
+      </c>
+      <c r="I15" s="17">
+        <f t="shared" si="0"/>
         <v>6.5807777777777767</v>
       </c>
-      <c r="H15" s="18">
+      <c r="J15" s="18">
         <f t="shared" si="0"/>
         <v>5.7406888888888883</v>
       </c>
-      <c r="I15" s="18">
+      <c r="K15" s="18">
         <f t="shared" si="0"/>
         <v>6.3639000000000001</v>
       </c>
-      <c r="J15" s="16">
+      <c r="L15" s="16">
         <f t="shared" si="0"/>
         <v>6.573666666666667</v>
       </c>
-      <c r="K15" s="17">
+      <c r="M15" s="17">
         <f t="shared" si="0"/>
         <v>5.7907222222222225</v>
       </c>
-      <c r="L15" s="18">
+      <c r="N15" s="18">
         <f t="shared" si="0"/>
         <v>5.8179999999999996</v>
       </c>
-      <c r="M15" s="18">
+      <c r="O15" s="18">
         <f t="shared" si="0"/>
         <v>5.5526888888888886</v>
       </c>
-      <c r="N15" s="16">
+      <c r="P15" s="16">
         <f t="shared" si="0"/>
         <v>7.5725333333333333</v>
       </c>
-      <c r="O15" s="17">
+      <c r="Q15" s="17">
         <f t="shared" si="0"/>
         <v>5.6041222222222213</v>
       </c>
-      <c r="P15" s="19">
+      <c r="R15" s="19">
         <f t="shared" si="0"/>
         <v>10.134733333333333</v>
       </c>
-      <c r="Q15" s="17">
+      <c r="S15" s="17">
         <f t="shared" si="0"/>
         <v>6.6618222222222219</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" s="31" t="s">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B16" s="25" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="2">
+        <v>1577.3805</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1199.7697000000001</v>
+      </c>
+      <c r="F16" s="7">
         <v>19.510200000000001</v>
       </c>
-      <c r="E16" s="8">
+      <c r="G16" s="8">
         <v>24.586500000000001</v>
       </c>
-      <c r="F16" s="7">
+      <c r="H16" s="7">
         <v>9.4801000000000002</v>
       </c>
-      <c r="G16" s="9">
+      <c r="I16" s="9">
         <v>5.7995999999999999</v>
       </c>
-      <c r="H16" s="9">
+      <c r="J16" s="9">
         <v>10.0245</v>
       </c>
-      <c r="I16" s="8">
+      <c r="K16" s="8">
         <v>5.8151000000000002</v>
       </c>
-      <c r="J16" s="7">
+      <c r="L16" s="7">
         <v>9.7077000000000009</v>
       </c>
-      <c r="K16" s="9">
+      <c r="M16" s="9">
         <v>6.0500999999999996</v>
       </c>
-      <c r="L16" s="9">
+      <c r="N16" s="9">
         <v>10.3523</v>
       </c>
-      <c r="M16" s="8">
+      <c r="O16" s="8">
         <v>6.0045000000000002</v>
       </c>
-      <c r="N16" s="7">
+      <c r="P16" s="7">
         <v>8.8854000000000006</v>
       </c>
-      <c r="O16" s="9">
+      <c r="Q16" s="9">
         <v>5.7096</v>
       </c>
-      <c r="P16" s="9">
+      <c r="R16" s="9">
         <v>12.6065</v>
       </c>
-      <c r="Q16" s="8">
+      <c r="S16" s="8">
         <v>6.5685000000000002</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="32"/>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B17" s="26"/>
       <c r="C17" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17">
+        <v>550.54769999999996</v>
+      </c>
+      <c r="E17">
+        <v>715.91409999999996</v>
+      </c>
+      <c r="F17" s="10">
         <v>17.152000000000001</v>
       </c>
-      <c r="E17" s="11">
+      <c r="G17" s="11">
         <v>19.156400000000001</v>
       </c>
-      <c r="F17" s="10">
+      <c r="H17" s="10">
         <v>7.5785999999999998</v>
       </c>
-      <c r="G17" s="12">
+      <c r="I17" s="12">
         <v>3.9401000000000002</v>
       </c>
-      <c r="H17" s="12">
+      <c r="J17" s="12">
         <v>7.1814</v>
       </c>
-      <c r="I17" s="11">
+      <c r="K17" s="11">
         <v>3.5247000000000002</v>
       </c>
-      <c r="J17" s="10">
+      <c r="L17" s="10">
         <v>6.4149000000000003</v>
       </c>
-      <c r="K17" s="12">
+      <c r="M17" s="12">
         <v>3.7139000000000002</v>
       </c>
-      <c r="L17" s="12">
+      <c r="N17" s="12">
         <v>7.2337999999999996</v>
       </c>
-      <c r="M17" s="11">
+      <c r="O17" s="11">
         <v>3.6772</v>
       </c>
-      <c r="N17" s="10">
+      <c r="P17" s="10">
         <v>7.3989000000000003</v>
       </c>
-      <c r="O17" s="12">
+      <c r="Q17" s="12">
         <v>3.7443</v>
       </c>
-      <c r="P17" s="12">
+      <c r="R17" s="12">
         <v>8.6593</v>
       </c>
-      <c r="Q17" s="11">
+      <c r="S17" s="11">
         <v>5.0378999999999996</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="32"/>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B18" s="26"/>
       <c r="C18" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18">
+        <v>1230.2163</v>
+      </c>
+      <c r="E18">
+        <v>792.07839999999999</v>
+      </c>
+      <c r="F18" s="10">
         <v>17.435099999999998</v>
       </c>
-      <c r="E18" s="11">
+      <c r="G18" s="11">
         <v>17.072500000000002</v>
       </c>
-      <c r="F18" s="10">
+      <c r="H18" s="10">
         <v>6.1877000000000004</v>
       </c>
-      <c r="G18" s="12">
+      <c r="I18" s="12">
         <v>4.0914000000000001</v>
       </c>
-      <c r="H18" s="12">
+      <c r="J18" s="12">
         <v>11.4697</v>
       </c>
-      <c r="I18" s="11">
+      <c r="K18" s="11">
         <v>3.6663000000000001</v>
       </c>
-      <c r="J18" s="10">
+      <c r="L18" s="10">
         <v>10.834</v>
       </c>
-      <c r="K18" s="12">
+      <c r="M18" s="12">
         <v>3.7793000000000001</v>
       </c>
-      <c r="L18" s="12">
+      <c r="N18" s="12">
         <v>11.8544</v>
       </c>
-      <c r="M18" s="11">
+      <c r="O18" s="11">
         <v>3.8153999999999999</v>
       </c>
-      <c r="N18" s="10">
+      <c r="P18" s="10">
         <v>11.0352</v>
       </c>
-      <c r="O18" s="12">
+      <c r="Q18" s="12">
         <v>3.6692999999999998</v>
       </c>
-      <c r="P18" s="12">
+      <c r="R18" s="12">
         <v>13.4208</v>
       </c>
-      <c r="Q18" s="11">
+      <c r="S18" s="11">
         <v>4.5228000000000002</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="32"/>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B19" s="26"/>
       <c r="C19" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19">
+        <v>625.43169999999998</v>
+      </c>
+      <c r="E19">
+        <v>933.94090000000006</v>
+      </c>
+      <c r="F19" s="10">
         <v>21.404499999999999</v>
       </c>
-      <c r="E19" s="11">
+      <c r="G19" s="11">
         <v>25.595199999999998</v>
       </c>
-      <c r="F19" s="10">
+      <c r="H19" s="10">
         <v>4.1031000000000004</v>
       </c>
-      <c r="G19" s="12">
+      <c r="I19" s="12">
         <v>5.2232000000000003</v>
       </c>
-      <c r="H19" s="12">
+      <c r="J19" s="12">
         <v>3.9958999999999998</v>
       </c>
-      <c r="I19" s="11">
+      <c r="K19" s="11">
         <v>5.1233000000000004</v>
       </c>
-      <c r="J19" s="10">
+      <c r="L19" s="10">
         <v>4.8121999999999998</v>
       </c>
-      <c r="K19" s="12">
+      <c r="M19" s="12">
         <v>5.0956000000000001</v>
       </c>
-      <c r="L19" s="12">
+      <c r="N19" s="12">
         <v>4.2687999999999997</v>
       </c>
-      <c r="M19" s="11">
+      <c r="O19" s="11">
         <v>5.0015000000000001</v>
       </c>
-      <c r="N19" s="10">
+      <c r="P19" s="10">
         <v>5.7196999999999996</v>
       </c>
-      <c r="O19" s="12">
+      <c r="Q19" s="12">
         <v>4.7160000000000002</v>
       </c>
-      <c r="P19" s="12">
+      <c r="R19" s="12">
         <v>6.2194000000000003</v>
       </c>
-      <c r="Q19" s="11">
+      <c r="S19" s="11">
         <v>5.8510999999999997</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="32"/>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B20" s="26"/>
       <c r="C20" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20">
+        <v>674.89570000000003</v>
+      </c>
+      <c r="E20">
+        <v>775.7269</v>
+      </c>
+      <c r="F20" s="10">
         <v>22.099299999999999</v>
       </c>
-      <c r="E20" s="11">
+      <c r="G20" s="11">
         <v>21.645</v>
       </c>
-      <c r="F20" s="12">
+      <c r="H20" s="12">
         <v>12.050599999999999</v>
       </c>
-      <c r="G20" s="12">
+      <c r="I20" s="12">
         <v>3.3936999999999999</v>
       </c>
-      <c r="H20" s="12">
+      <c r="J20" s="12">
         <v>11.9215</v>
       </c>
-      <c r="I20" s="11">
+      <c r="K20" s="11">
         <v>3.6848000000000001</v>
       </c>
-      <c r="J20" s="10">
+      <c r="L20" s="10">
         <v>12.182399999999999</v>
       </c>
-      <c r="K20" s="12">
+      <c r="M20" s="12">
         <v>3.8570000000000002</v>
       </c>
-      <c r="L20" s="12">
+      <c r="N20" s="12">
         <v>12.2585</v>
       </c>
-      <c r="M20" s="11">
+      <c r="O20" s="11">
         <v>4.0084999999999997</v>
       </c>
-      <c r="N20" s="10">
+      <c r="P20" s="10">
         <v>12.0623</v>
       </c>
-      <c r="O20" s="12">
+      <c r="Q20" s="12">
         <v>3.7955999999999999</v>
       </c>
-      <c r="P20" s="12">
+      <c r="R20" s="12">
         <v>11.024100000000001</v>
       </c>
-      <c r="Q20" s="11">
+      <c r="S20" s="11">
         <v>3.9596</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B21" s="32"/>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B21" s="26"/>
       <c r="C21" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21">
+        <v>2282.3031999999998</v>
+      </c>
+      <c r="E21">
+        <v>1182.3946000000001</v>
+      </c>
+      <c r="F21" s="10">
         <v>35.577800000000003</v>
       </c>
-      <c r="E21" s="11">
+      <c r="G21" s="11">
         <v>38.195399999999999</v>
       </c>
-      <c r="F21" s="10">
+      <c r="H21" s="10">
         <v>9.6591000000000005</v>
       </c>
-      <c r="G21" s="12">
+      <c r="I21" s="12">
         <v>6.9629000000000003</v>
       </c>
-      <c r="H21" s="12">
+      <c r="J21" s="12">
         <v>10.741899999999999</v>
       </c>
-      <c r="I21" s="11">
+      <c r="K21" s="11">
         <v>4.3586</v>
       </c>
-      <c r="J21" s="10">
+      <c r="L21" s="10">
         <v>9.0980000000000008</v>
       </c>
-      <c r="K21" s="12">
+      <c r="M21" s="12">
         <v>6.6542000000000003</v>
       </c>
-      <c r="L21" s="12">
+      <c r="N21" s="12">
         <v>10.397</v>
       </c>
-      <c r="M21" s="11">
+      <c r="O21" s="11">
         <v>6.3644999999999996</v>
       </c>
-      <c r="N21" s="10">
+      <c r="P21" s="10">
         <v>8.6968999999999994</v>
       </c>
-      <c r="O21" s="12">
+      <c r="Q21" s="12">
         <v>6.0517000000000003</v>
       </c>
-      <c r="P21" s="12">
+      <c r="R21" s="12">
         <v>9.6264000000000003</v>
       </c>
-      <c r="Q21" s="11">
+      <c r="S21" s="11">
         <v>7.8384999999999998</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B22" s="32"/>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B22" s="26"/>
       <c r="C22" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22">
+        <v>616.1866</v>
+      </c>
+      <c r="E22">
+        <v>1040.1365000000001</v>
+      </c>
+      <c r="F22" s="10">
         <v>41.508299999999998</v>
       </c>
-      <c r="E22" s="11">
+      <c r="G22" s="11">
         <v>42.203899999999997</v>
       </c>
-      <c r="F22" s="10">
+      <c r="H22" s="10">
         <v>6.1943999999999999</v>
       </c>
-      <c r="G22" s="12">
+      <c r="I22" s="12">
         <v>6.4965999999999999</v>
       </c>
-      <c r="H22" s="12">
+      <c r="J22" s="12">
         <v>6.6238999999999999</v>
       </c>
-      <c r="I22" s="11">
+      <c r="K22" s="11">
         <v>6.4550999999999998</v>
       </c>
-      <c r="J22" s="10">
+      <c r="L22" s="10">
         <v>7.0220000000000002</v>
       </c>
-      <c r="K22" s="12">
+      <c r="M22" s="12">
         <v>6.8677999999999999</v>
       </c>
-      <c r="L22" s="12">
+      <c r="N22" s="12">
         <v>7.4859</v>
       </c>
-      <c r="M22" s="11">
+      <c r="O22" s="11">
         <v>7.2760999999999996</v>
       </c>
-      <c r="N22" s="10">
+      <c r="P22" s="10">
         <v>9.2472999999999992</v>
       </c>
-      <c r="O22" s="12">
+      <c r="Q22" s="12">
         <v>7.0589000000000004</v>
       </c>
-      <c r="P22" s="12">
+      <c r="R22" s="12">
         <v>10.7371</v>
       </c>
-      <c r="Q22" s="11">
+      <c r="S22" s="11">
         <v>8.4207999999999998</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="32"/>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="26"/>
       <c r="C23" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23">
+        <v>949.9203</v>
+      </c>
+      <c r="E23">
+        <v>945.89589999999998</v>
+      </c>
+      <c r="F23" s="10">
         <v>27.623100000000001</v>
       </c>
-      <c r="E23" s="11">
+      <c r="G23" s="11">
         <v>36.150100000000002</v>
       </c>
-      <c r="F23" s="10">
+      <c r="H23" s="10">
         <v>4.9349999999999996</v>
       </c>
-      <c r="G23" s="12">
+      <c r="I23" s="12">
         <v>7.8406000000000002</v>
       </c>
-      <c r="H23" s="12">
+      <c r="J23" s="12">
         <v>4.4421999999999997</v>
       </c>
-      <c r="I23" s="11">
+      <c r="K23" s="11">
         <v>6.9725000000000001</v>
       </c>
-      <c r="J23" s="10">
+      <c r="L23" s="10">
         <v>5.1417000000000002</v>
       </c>
-      <c r="K23" s="12">
+      <c r="M23" s="12">
         <v>7.5467000000000004</v>
       </c>
-      <c r="L23" s="12">
+      <c r="N23" s="12">
         <v>4.5373000000000001</v>
       </c>
-      <c r="M23" s="11">
+      <c r="O23" s="11">
         <v>6.6073000000000004</v>
       </c>
-      <c r="N23" s="10">
+      <c r="P23" s="10">
         <v>5.9424000000000001</v>
       </c>
-      <c r="O23" s="12">
+      <c r="Q23" s="12">
         <v>6.1997999999999998</v>
       </c>
-      <c r="P23" s="12">
+      <c r="R23" s="12">
         <v>8.3137000000000008</v>
       </c>
-      <c r="Q23" s="11">
+      <c r="S23" s="11">
         <v>7.2359999999999998</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="32"/>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="26"/>
       <c r="C24" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24">
+        <v>1426.2719999999999</v>
+      </c>
+      <c r="E24">
+        <v>843.14850000000001</v>
+      </c>
+      <c r="F24" s="10">
         <v>16.4725</v>
       </c>
-      <c r="E24" s="11">
+      <c r="G24" s="11">
         <v>18.293099999999999</v>
       </c>
-      <c r="F24" s="10">
+      <c r="H24" s="10">
         <v>6.7008000000000001</v>
       </c>
-      <c r="G24" s="12">
+      <c r="I24" s="12">
         <v>3.6524000000000001</v>
       </c>
-      <c r="H24" s="12">
+      <c r="J24" s="12">
         <v>5.9278000000000004</v>
       </c>
-      <c r="I24" s="11">
+      <c r="K24" s="11">
         <v>3.6494</v>
       </c>
-      <c r="J24" s="10">
+      <c r="L24" s="10">
         <v>7.0419</v>
       </c>
-      <c r="K24" s="12">
+      <c r="M24" s="12">
         <v>4.0312000000000001</v>
       </c>
-      <c r="L24" s="12">
+      <c r="N24" s="12">
         <v>6.06</v>
       </c>
-      <c r="M24" s="11">
+      <c r="O24" s="11">
         <v>3.8296000000000001</v>
       </c>
-      <c r="N24" s="10">
+      <c r="P24" s="10">
         <v>7.0296000000000003</v>
       </c>
-      <c r="O24" s="12">
+      <c r="Q24" s="12">
         <v>3.4447000000000001</v>
       </c>
-      <c r="P24" s="12">
+      <c r="R24" s="12">
         <v>11.639099999999999</v>
       </c>
-      <c r="Q24" s="11">
+      <c r="S24" s="11">
         <v>4.5247999999999999</v>
       </c>
     </row>
-    <row r="25" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="33"/>
+    <row r="25" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="27"/>
       <c r="C25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D25" s="1">
+        <v>1889.8598999999999</v>
+      </c>
+      <c r="E25" s="1">
+        <v>920.27359999999999</v>
+      </c>
+      <c r="F25" s="13">
         <v>13.1075</v>
       </c>
-      <c r="E25" s="14">
+      <c r="G25" s="14">
         <v>16.594799999999999</v>
       </c>
-      <c r="F25" s="13">
+      <c r="H25" s="13">
         <v>2.1724000000000001</v>
       </c>
-      <c r="G25" s="15">
+      <c r="I25" s="15">
         <v>4.4269999999999996</v>
       </c>
-      <c r="H25" s="15">
+      <c r="J25" s="15">
         <v>2.8056000000000001</v>
       </c>
-      <c r="I25" s="14">
+      <c r="K25" s="14">
         <v>4.0418000000000003</v>
       </c>
-      <c r="J25" s="13">
+      <c r="L25" s="13">
         <v>3.0297000000000001</v>
       </c>
-      <c r="K25" s="15">
+      <c r="M25" s="15">
         <v>4.2751999999999999</v>
       </c>
-      <c r="L25" s="15">
+      <c r="N25" s="15">
         <v>3.0705</v>
       </c>
-      <c r="M25" s="14">
+      <c r="O25" s="14">
         <v>3.9986999999999999</v>
       </c>
-      <c r="N25" s="13">
+      <c r="P25" s="13">
         <v>4.7736000000000001</v>
       </c>
-      <c r="O25" s="15">
+      <c r="Q25" s="15">
         <v>4.1780999999999997</v>
       </c>
-      <c r="P25" s="15">
+      <c r="R25" s="15">
         <v>6.7962999999999996</v>
       </c>
-      <c r="Q25" s="14">
+      <c r="S25" s="14">
         <v>4.8756000000000004</v>
       </c>
     </row>
-    <row r="26" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D26" s="16">
-        <f t="shared" ref="D26:Q26" si="1">SUM(D16:D25)/10</f>
-        <v>23.189029999999995</v>
+        <f t="shared" ref="D26:S26" si="1">SUM(D16:D25)/10</f>
+        <v>1182.3013900000001</v>
       </c>
       <c r="E26" s="17">
         <f t="shared" si="1"/>
-        <v>25.949290000000001</v>
+        <v>934.92791</v>
       </c>
       <c r="F26" s="16">
         <f t="shared" si="1"/>
-        <v>6.9061800000000009</v>
+        <v>23.189029999999995</v>
       </c>
       <c r="G26" s="17">
         <f t="shared" si="1"/>
-        <v>5.1827500000000004</v>
+        <v>25.949290000000001</v>
       </c>
       <c r="H26" s="16">
         <f t="shared" si="1"/>
-        <v>7.513440000000001</v>
+        <v>6.9061800000000009</v>
       </c>
       <c r="I26" s="17">
         <f t="shared" si="1"/>
+        <v>5.1827500000000004</v>
+      </c>
+      <c r="J26" s="16">
+        <f t="shared" si="1"/>
+        <v>7.513440000000001</v>
+      </c>
+      <c r="K26" s="17">
+        <f t="shared" si="1"/>
         <v>4.7291599999999994</v>
       </c>
-      <c r="J26" s="19">
+      <c r="L26" s="19">
         <f t="shared" si="1"/>
         <v>7.5284499999999994</v>
       </c>
-      <c r="K26" s="17">
+      <c r="M26" s="17">
         <f t="shared" si="1"/>
         <v>5.1870999999999992</v>
       </c>
-      <c r="L26" s="19">
+      <c r="N26" s="19">
         <f t="shared" si="1"/>
         <v>7.7518499999999992</v>
       </c>
-      <c r="M26" s="17">
+      <c r="O26" s="17">
         <f t="shared" si="1"/>
         <v>5.0583299999999998</v>
       </c>
-      <c r="N26" s="19">
+      <c r="P26" s="19">
         <f t="shared" si="1"/>
         <v>8.079130000000001</v>
       </c>
-      <c r="O26" s="17">
+      <c r="Q26" s="17">
         <f t="shared" si="1"/>
         <v>4.8567999999999998</v>
       </c>
-      <c r="P26" s="19">
+      <c r="R26" s="19">
         <f t="shared" si="1"/>
         <v>9.9042700000000004</v>
       </c>
-      <c r="Q26" s="17">
+      <c r="S26" s="17">
         <f t="shared" si="1"/>
         <v>5.8835600000000001</v>
       </c>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="31" t="s">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B27" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="2">
+        <v>2751.1170999999999</v>
+      </c>
+      <c r="E27" s="2">
+        <v>3407.5169000000001</v>
+      </c>
+      <c r="F27" s="7">
         <v>24.516100000000002</v>
       </c>
-      <c r="E27" s="8">
+      <c r="G27" s="8">
         <v>28.6495</v>
       </c>
-      <c r="F27" s="7">
+      <c r="H27" s="7">
         <v>24.099699999999999</v>
       </c>
-      <c r="G27" s="9">
+      <c r="I27" s="9">
         <v>23.979600000000001</v>
       </c>
-      <c r="H27" s="9">
+      <c r="J27" s="9">
         <v>21.7912</v>
       </c>
-      <c r="I27" s="8">
+      <c r="K27" s="8">
         <v>22.681100000000001</v>
       </c>
-      <c r="J27" s="7">
+      <c r="L27" s="7">
         <v>24.099699999999999</v>
       </c>
-      <c r="K27" s="9">
+      <c r="M27" s="9">
         <v>23.979600000000001</v>
       </c>
-      <c r="L27" s="9">
+      <c r="N27" s="9">
         <v>21.7912</v>
       </c>
-      <c r="M27" s="8">
+      <c r="O27" s="8">
         <v>22.681100000000001</v>
       </c>
-      <c r="N27" s="7">
+      <c r="P27" s="7">
         <v>31.872800000000002</v>
       </c>
-      <c r="O27" s="9">
+      <c r="Q27" s="9">
         <v>25.048100000000002</v>
       </c>
-      <c r="P27" s="9">
+      <c r="R27" s="9">
         <v>19.585599999999999</v>
       </c>
-      <c r="Q27" s="8">
+      <c r="S27" s="8">
         <v>20.312200000000001</v>
       </c>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="32"/>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B28" s="26"/>
       <c r="C28" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="10">
+        <v>22</v>
+      </c>
+      <c r="D28">
+        <v>2282.3031999999998</v>
+      </c>
+      <c r="E28">
+        <v>1182.3946000000001</v>
+      </c>
+      <c r="F28" s="10">
         <v>35.577800000000003</v>
       </c>
-      <c r="E28" s="11">
+      <c r="G28" s="11">
         <v>38.195399999999999</v>
       </c>
-      <c r="F28" s="10">
+      <c r="H28" s="10">
         <v>9.0980000000000008</v>
       </c>
-      <c r="G28" s="12">
+      <c r="I28" s="12">
         <v>6.6542000000000003</v>
       </c>
-      <c r="H28" s="12">
+      <c r="J28" s="12">
         <v>10.397</v>
       </c>
-      <c r="I28" s="11">
+      <c r="K28" s="11">
         <v>6.3644999999999996</v>
       </c>
-      <c r="J28" s="10">
+      <c r="L28" s="10">
         <v>9.0980000000000008</v>
       </c>
-      <c r="K28" s="12">
+      <c r="M28" s="12">
         <v>6.6542000000000003</v>
       </c>
-      <c r="L28" s="12">
+      <c r="N28" s="12">
         <v>10.397</v>
       </c>
-      <c r="M28" s="11">
+      <c r="O28" s="11">
         <v>6.3644999999999996</v>
       </c>
-      <c r="N28" s="10">
+      <c r="P28" s="10">
         <v>22.5945</v>
       </c>
-      <c r="O28" s="12">
+      <c r="Q28" s="12">
         <v>13.5779</v>
       </c>
-      <c r="P28" s="12">
+      <c r="R28" s="12">
         <v>31.0091</v>
       </c>
-      <c r="Q28" s="11">
+      <c r="S28" s="11">
         <v>8.1875</v>
       </c>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="32"/>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B29" s="26"/>
       <c r="C29" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29">
+        <v>4381.1242000000002</v>
+      </c>
+      <c r="E29">
+        <v>4228.5518000000002</v>
+      </c>
+      <c r="F29" s="10">
         <v>16.888000000000002</v>
       </c>
-      <c r="E29" s="11">
+      <c r="G29" s="11">
         <v>8.6329999999999991</v>
       </c>
-      <c r="F29" s="10">
+      <c r="H29" s="10">
         <v>1.6156999999999999</v>
       </c>
-      <c r="G29" s="12">
+      <c r="I29" s="12">
         <v>11.8727</v>
       </c>
-      <c r="H29" s="12">
+      <c r="J29" s="12">
         <v>10.8146</v>
       </c>
-      <c r="I29" s="11">
+      <c r="K29" s="11">
         <v>8.4617000000000004</v>
       </c>
-      <c r="J29" s="10">
+      <c r="L29" s="10">
         <v>1.6156999999999999</v>
       </c>
-      <c r="K29" s="12">
+      <c r="M29" s="12">
         <v>11.8727</v>
       </c>
-      <c r="L29" s="12">
+      <c r="N29" s="12">
         <v>10.8146</v>
       </c>
-      <c r="M29" s="11">
+      <c r="O29" s="11">
         <v>8.4617000000000004</v>
       </c>
-      <c r="N29" s="10">
+      <c r="P29" s="10">
         <v>12.3986</v>
       </c>
-      <c r="O29" s="12">
+      <c r="Q29" s="12">
         <v>13.6015</v>
       </c>
-      <c r="P29" s="12">
+      <c r="R29" s="12">
         <v>9.1115999999999993</v>
       </c>
-      <c r="Q29" s="11">
+      <c r="S29" s="11">
         <v>7.3815999999999997</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B30" s="32"/>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B30" s="26"/>
       <c r="C30" t="s">
         <v>3</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D30">
+        <v>3748.3908000000001</v>
+      </c>
+      <c r="E30">
+        <v>3282.1078000000002</v>
+      </c>
+      <c r="F30" s="10">
         <v>17.375800000000002</v>
       </c>
-      <c r="E30" s="11">
+      <c r="G30" s="11">
         <v>6.9199000000000002</v>
       </c>
-      <c r="F30" s="10">
+      <c r="H30" s="10">
         <v>9.7042999999999999</v>
       </c>
-      <c r="G30" s="12">
+      <c r="I30" s="12">
         <v>6.8817000000000004</v>
       </c>
-      <c r="H30" s="12">
+      <c r="J30" s="12">
         <v>13.8003</v>
       </c>
-      <c r="I30" s="11">
+      <c r="K30" s="11">
         <v>2.7940999999999998</v>
       </c>
-      <c r="J30" s="10">
+      <c r="L30" s="10">
         <v>9.7042999999999999</v>
       </c>
-      <c r="K30" s="12">
+      <c r="M30" s="12">
         <v>6.8817000000000004</v>
       </c>
-      <c r="L30" s="12">
+      <c r="N30" s="12">
         <v>13.8003</v>
       </c>
-      <c r="M30" s="11">
+      <c r="O30" s="11">
         <v>2.7940999999999998</v>
       </c>
-      <c r="N30" s="10">
+      <c r="P30" s="10">
         <v>7.1182999999999996</v>
       </c>
-      <c r="O30" s="12">
+      <c r="Q30" s="12">
         <v>9.3779000000000003</v>
       </c>
-      <c r="P30" s="12">
+      <c r="R30" s="12">
         <v>9.6632999999999996</v>
       </c>
-      <c r="Q30" s="11">
+      <c r="S30" s="11">
         <v>0.61168</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="32"/>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B31" s="26"/>
       <c r="C31" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D31">
+        <v>2534.6154999999999</v>
+      </c>
+      <c r="E31">
+        <v>2135.1514999999999</v>
+      </c>
+      <c r="F31" s="10">
         <v>3.8386999999999998</v>
       </c>
-      <c r="E31" s="11">
+      <c r="G31" s="11">
         <v>6.1504000000000003</v>
       </c>
-      <c r="F31" s="10">
+      <c r="H31" s="10">
         <v>4.0777000000000001</v>
       </c>
-      <c r="G31" s="12">
+      <c r="I31" s="12">
         <v>5.3647</v>
       </c>
-      <c r="H31" s="12">
+      <c r="J31" s="12">
         <v>3.8147000000000002</v>
       </c>
-      <c r="I31" s="11">
+      <c r="K31" s="11">
         <v>5.7195999999999998</v>
       </c>
-      <c r="J31" s="10">
+      <c r="L31" s="10">
         <v>4.0777000000000001</v>
       </c>
-      <c r="K31" s="12">
+      <c r="M31" s="12">
         <v>5.3647</v>
       </c>
-      <c r="L31" s="12">
+      <c r="N31" s="12">
         <v>3.8147000000000002</v>
       </c>
-      <c r="M31" s="11">
+      <c r="O31" s="11">
         <v>5.7195999999999998</v>
       </c>
-      <c r="N31" s="10">
+      <c r="P31" s="10">
         <v>13.264200000000001</v>
       </c>
-      <c r="O31" s="12">
+      <c r="Q31" s="12">
         <v>8.3228000000000009</v>
       </c>
-      <c r="P31" s="12">
+      <c r="R31" s="12">
         <v>1.7384999999999999</v>
       </c>
-      <c r="Q31" s="11">
+      <c r="S31" s="11">
         <v>3.3567999999999998</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B32" s="32"/>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B32" s="26"/>
       <c r="C32" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="10">
+      <c r="D32">
+        <v>4321.4444000000003</v>
+      </c>
+      <c r="E32">
+        <v>4355.2654000000002</v>
+      </c>
+      <c r="F32" s="10">
         <v>9.8919999999999995</v>
       </c>
-      <c r="E32" s="11">
+      <c r="G32" s="11">
         <v>17.6081</v>
       </c>
-      <c r="F32" s="10">
+      <c r="H32" s="10">
         <v>9.2612000000000005</v>
       </c>
-      <c r="G32" s="12">
+      <c r="I32" s="12">
         <v>19.231300000000001</v>
       </c>
-      <c r="H32" s="12">
+      <c r="J32" s="12">
         <v>4.5425000000000004</v>
       </c>
-      <c r="I32" s="11">
+      <c r="K32" s="11">
         <v>16.572600000000001</v>
       </c>
-      <c r="J32" s="10">
+      <c r="L32" s="10">
         <v>9.2612000000000005</v>
       </c>
-      <c r="K32" s="12">
+      <c r="M32" s="12">
         <v>19.231300000000001</v>
       </c>
-      <c r="L32" s="12">
+      <c r="N32" s="12">
         <v>4.5425000000000004</v>
       </c>
-      <c r="M32" s="11">
+      <c r="O32" s="11">
         <v>16.572600000000001</v>
       </c>
-      <c r="N32" s="10">
+      <c r="P32" s="10">
         <v>18.748200000000001</v>
       </c>
-      <c r="O32" s="12">
+      <c r="Q32" s="12">
         <v>19.341899999999999</v>
       </c>
-      <c r="P32" s="12">
+      <c r="R32" s="12">
         <v>8.8446999999999996</v>
       </c>
-      <c r="Q32" s="11">
+      <c r="S32" s="11">
         <v>9.33</v>
       </c>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B33" s="32"/>
+    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B33" s="26"/>
       <c r="C33" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D33">
+        <v>5255.1144000000004</v>
+      </c>
+      <c r="E33">
+        <v>5669.9522999999999</v>
+      </c>
+      <c r="F33" s="10">
         <v>51.776499999999999</v>
       </c>
-      <c r="E33" s="11">
+      <c r="G33" s="11">
         <v>5.7306999999999997</v>
       </c>
-      <c r="F33" s="10">
+      <c r="H33" s="10">
         <v>21.876899999999999</v>
       </c>
-      <c r="G33" s="12">
+      <c r="I33" s="12">
         <v>8.1357999999999997</v>
       </c>
-      <c r="H33" s="12">
+      <c r="J33" s="12">
         <v>22.810400000000001</v>
       </c>
-      <c r="I33" s="11">
+      <c r="K33" s="11">
         <v>0.65000999999999998</v>
       </c>
-      <c r="J33" s="10">
+      <c r="L33" s="10">
         <v>21.876899999999999</v>
       </c>
-      <c r="K33" s="12">
+      <c r="M33" s="12">
         <v>8.1357999999999997</v>
       </c>
-      <c r="L33" s="12">
+      <c r="N33" s="12">
         <v>22.810400000000001</v>
       </c>
-      <c r="M33" s="11">
+      <c r="O33" s="11">
         <v>0.65000999999999998</v>
       </c>
-      <c r="N33" s="10">
+      <c r="P33" s="10">
         <v>27.830500000000001</v>
       </c>
-      <c r="O33" s="12">
+      <c r="Q33" s="12">
         <v>16.521999999999998</v>
       </c>
-      <c r="P33" s="12">
+      <c r="R33" s="12">
         <v>8.8048999999999999</v>
       </c>
-      <c r="Q33" s="11">
+      <c r="S33" s="11">
         <v>3.3877999999999998E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B34" s="32"/>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B34" s="26"/>
       <c r="C34" t="s">
-        <v>23</v>
-      </c>
-      <c r="D34" s="10">
+        <v>21</v>
+      </c>
+      <c r="D34">
+        <v>6921.3692000000001</v>
+      </c>
+      <c r="E34">
+        <v>11035.723900000001</v>
+      </c>
+      <c r="F34" s="10">
         <v>26.3611</v>
       </c>
-      <c r="E34" s="11">
+      <c r="G34" s="11">
         <v>0.55650999999999995</v>
       </c>
-      <c r="F34" s="10">
+      <c r="H34" s="10">
         <v>5.3124000000000002</v>
       </c>
-      <c r="G34" s="12">
+      <c r="I34" s="12">
         <v>10.8703</v>
       </c>
-      <c r="H34" s="12">
+      <c r="J34" s="12">
         <v>7.4404000000000003</v>
       </c>
-      <c r="I34" s="11">
+      <c r="K34" s="11">
         <v>7.1334999999999997</v>
       </c>
-      <c r="J34" s="10">
+      <c r="L34" s="10">
         <v>5.3124000000000002</v>
       </c>
-      <c r="K34" s="12">
+      <c r="M34" s="12">
         <v>10.8703</v>
       </c>
-      <c r="L34" s="12">
+      <c r="N34" s="12">
         <v>7.4404000000000003</v>
       </c>
-      <c r="M34" s="11">
+      <c r="O34" s="11">
         <v>7.1334999999999997</v>
       </c>
-      <c r="N34" s="10">
+      <c r="P34" s="10">
         <v>4.1058000000000003</v>
       </c>
-      <c r="O34" s="12">
+      <c r="Q34" s="12">
         <v>9.7471999999999994</v>
       </c>
-      <c r="P34" s="12">
+      <c r="R34" s="12">
         <v>12.9803</v>
       </c>
-      <c r="Q34" s="11">
+      <c r="S34" s="11">
         <v>0.96741999999999995</v>
       </c>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B35" s="32"/>
+    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B35" s="26"/>
       <c r="C35" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="10">
+      <c r="D35">
+        <v>3726.3222000000001</v>
+      </c>
+      <c r="E35">
+        <v>1930.1717000000001</v>
+      </c>
+      <c r="F35" s="10">
         <v>6.3155999999999999</v>
       </c>
-      <c r="E35" s="11">
+      <c r="G35" s="11">
         <v>9.6661999999999999</v>
       </c>
-      <c r="F35" s="10">
+      <c r="H35" s="10">
         <v>5.5168999999999997</v>
       </c>
-      <c r="G35" s="12">
+      <c r="I35" s="12">
         <v>10.2943</v>
       </c>
-      <c r="H35" s="12">
+      <c r="J35" s="12">
         <v>5.0214999999999996</v>
       </c>
-      <c r="I35" s="11">
+      <c r="K35" s="11">
         <v>10.2034</v>
       </c>
-      <c r="J35" s="10">
+      <c r="L35" s="10">
         <v>5.5168999999999997</v>
       </c>
-      <c r="K35" s="12">
+      <c r="M35" s="12">
         <v>10.2943</v>
       </c>
-      <c r="L35" s="12">
+      <c r="N35" s="12">
         <v>5.0214999999999996</v>
       </c>
-      <c r="M35" s="11">
+      <c r="O35" s="11">
         <v>10.2034</v>
       </c>
-      <c r="N35" s="10">
+      <c r="P35" s="10">
         <v>5.0728999999999997</v>
       </c>
-      <c r="O35" s="12">
+      <c r="Q35" s="12">
         <v>10.2105</v>
       </c>
-      <c r="P35" s="12">
+      <c r="R35" s="12">
         <v>9.7768999999999995</v>
       </c>
-      <c r="Q35" s="11">
+      <c r="S35" s="11">
         <v>10.8696</v>
       </c>
     </row>
-    <row r="36" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="33"/>
+    <row r="36" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="27"/>
       <c r="C36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D36" s="13">
+      <c r="D36" s="1">
+        <v>1081.9380000000001</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1397.9684999999999</v>
+      </c>
+      <c r="F36" s="13">
         <v>7.3684000000000003</v>
       </c>
-      <c r="E36" s="14">
+      <c r="G36" s="14">
         <v>7.9244000000000003</v>
       </c>
-      <c r="F36" s="13">
+      <c r="H36" s="13">
         <v>9.9684000000000008</v>
       </c>
-      <c r="G36" s="15">
+      <c r="I36" s="15">
         <v>9.3204999999999991</v>
       </c>
-      <c r="H36" s="15">
+      <c r="J36" s="15">
         <v>8.8717000000000006</v>
       </c>
-      <c r="I36" s="14">
+      <c r="K36" s="14">
         <v>9.0647000000000002</v>
       </c>
-      <c r="J36" s="13">
+      <c r="L36" s="13">
         <v>9.9684000000000008</v>
       </c>
-      <c r="K36" s="15">
+      <c r="M36" s="15">
         <v>9.3204999999999991</v>
       </c>
-      <c r="L36" s="15">
+      <c r="N36" s="15">
         <v>8.8717000000000006</v>
       </c>
-      <c r="M36" s="14">
+      <c r="O36" s="14">
         <v>9.0647000000000002</v>
       </c>
-      <c r="N36" s="13">
+      <c r="P36" s="13">
         <v>10.8413</v>
       </c>
-      <c r="O36" s="15">
+      <c r="Q36" s="15">
         <v>9.2133000000000003</v>
       </c>
-      <c r="P36" s="15">
+      <c r="R36" s="15">
         <v>9.7493999999999996</v>
       </c>
-      <c r="Q36" s="14">
+      <c r="S36" s="14">
         <v>9.3792000000000009</v>
       </c>
     </row>
-    <row r="37" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D37" s="16">
-        <f t="shared" ref="D37:Q37" si="2">SUM(D27:D36)/10</f>
-        <v>19.991</v>
+        <f t="shared" ref="D37:S37" si="2">SUM(D27:D36)/10</f>
+        <v>3700.373900000001</v>
       </c>
       <c r="E37" s="17">
         <f t="shared" si="2"/>
+        <v>3862.4804400000003</v>
+      </c>
+      <c r="F37" s="16">
+        <f t="shared" si="2"/>
+        <v>19.991</v>
+      </c>
+      <c r="G37" s="17">
+        <f t="shared" si="2"/>
         <v>13.003411</v>
       </c>
-      <c r="F37" s="19">
+      <c r="H37" s="19">
         <f t="shared" si="2"/>
         <v>10.053119999999998</v>
       </c>
-      <c r="G37" s="17">
+      <c r="I37" s="17">
         <f t="shared" si="2"/>
         <v>11.26051</v>
       </c>
-      <c r="H37" s="19">
+      <c r="J37" s="19">
         <f t="shared" si="2"/>
         <v>10.930430000000001</v>
       </c>
-      <c r="I37" s="17">
+      <c r="K37" s="17">
         <f t="shared" si="2"/>
         <v>8.9645210000000013</v>
       </c>
-      <c r="J37" s="19">
+      <c r="L37" s="19">
         <f t="shared" si="2"/>
         <v>10.053119999999998</v>
       </c>
-      <c r="K37" s="17">
+      <c r="M37" s="17">
         <f t="shared" si="2"/>
         <v>11.26051</v>
       </c>
-      <c r="L37" s="19">
+      <c r="N37" s="19">
         <f t="shared" si="2"/>
         <v>10.930430000000001</v>
       </c>
-      <c r="M37" s="17">
+      <c r="O37" s="17">
         <f t="shared" si="2"/>
         <v>8.9645210000000013</v>
       </c>
-      <c r="N37" s="19">
+      <c r="P37" s="19">
         <f t="shared" si="2"/>
         <v>15.384709999999998</v>
       </c>
-      <c r="O37" s="17">
+      <c r="Q37" s="17">
         <f t="shared" si="2"/>
         <v>13.496309999999999</v>
       </c>
-      <c r="P37" s="19">
+      <c r="R37" s="19">
         <f t="shared" si="2"/>
         <v>12.126429999999999</v>
       </c>
-      <c r="Q37" s="17">
+      <c r="S37" s="17">
         <f t="shared" si="2"/>
         <v>7.0429878000000006</v>
       </c>
     </row>
-    <row r="38" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
+    <row r="38" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F38" s="12"/>
       <c r="G38" s="12"/>
       <c r="H38" s="12"/>
@@ -2435,147 +2709,204 @@
       <c r="O38" s="12"/>
       <c r="P38" s="12"/>
       <c r="Q38" s="12"/>
-    </row>
-    <row r="39" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R38" s="12"/>
+      <c r="S38" s="12"/>
+    </row>
+    <row r="39" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D39" s="20">
         <f>SUM(D15,D26,D37)/3</f>
-        <v>23.558784074074072</v>
+        <v>2021.2773114814818</v>
       </c>
       <c r="E39" s="21">
-        <f t="shared" ref="E39:I39" si="3">SUM(E15,E26,E37)/3</f>
-        <v>23.596004037037037</v>
+        <f t="shared" ref="E39:K39" si="3">SUM(E15,E26,E37)/3</f>
+        <v>1985.4353388888892</v>
       </c>
       <c r="F39" s="20">
         <f>SUM(F15,F26,F37)/3</f>
-        <v>7.6185851851851849</v>
+        <v>23.558784074074072</v>
       </c>
       <c r="G39" s="21">
         <f t="shared" si="3"/>
+        <v>23.596004037037037</v>
+      </c>
+      <c r="H39" s="20">
+        <f>SUM(H15,H26,H37)/3</f>
+        <v>7.6185851851851849</v>
+      </c>
+      <c r="I39" s="21">
+        <f t="shared" si="3"/>
         <v>7.6746792592592596</v>
       </c>
-      <c r="H39" s="22">
+      <c r="J39" s="22">
         <f t="shared" si="3"/>
         <v>8.0615196296296308</v>
       </c>
-      <c r="I39" s="21">
+      <c r="K39" s="21">
         <f t="shared" si="3"/>
         <v>6.6858603333333333</v>
       </c>
-      <c r="J39" s="20">
-        <f>SUM(J15,J26,J37)/3</f>
+      <c r="L39" s="20">
+        <f>SUM(L15,L26,L37)/3</f>
         <v>8.0517455555555557</v>
       </c>
-      <c r="K39" s="21">
-        <f t="shared" ref="K39:Q39" si="4">SUM(K15,K26,K37)/3</f>
+      <c r="M39" s="21">
+        <f t="shared" ref="M39:S39" si="4">SUM(M15,M26,M37)/3</f>
         <v>7.4127774074074075</v>
       </c>
-      <c r="L39" s="22">
+      <c r="N39" s="22">
         <f t="shared" si="4"/>
         <v>8.16676</v>
       </c>
-      <c r="M39" s="21">
+      <c r="O39" s="21">
         <f t="shared" si="4"/>
         <v>6.5251799629629632</v>
       </c>
-      <c r="N39" s="20">
-        <f>SUM(N15,N26,N37)/3</f>
+      <c r="P39" s="20">
+        <f>SUM(P15,P26,P37)/3</f>
         <v>10.345457777777778</v>
       </c>
-      <c r="O39" s="21">
+      <c r="Q39" s="21">
         <f t="shared" si="4"/>
         <v>7.9857440740740735</v>
       </c>
-      <c r="P39" s="22">
+      <c r="R39" s="22">
         <f t="shared" si="4"/>
         <v>10.72181111111111</v>
       </c>
-      <c r="Q39" s="21">
+      <c r="S39" s="21">
         <f t="shared" si="4"/>
         <v>6.5294566740740736</v>
       </c>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="H41">
-        <f>F39/H39</f>
+    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="J41">
+        <f>H39/J39</f>
         <v>0.94505571346418771</v>
       </c>
-      <c r="I41">
-        <f>G39/I39</f>
+      <c r="K41">
+        <f>I39/K39</f>
         <v>1.1478970359276015</v>
       </c>
-      <c r="L41">
-        <f>J39/L39</f>
+      <c r="N41">
+        <f>L39/N39</f>
         <v>0.98591675959077474</v>
       </c>
-      <c r="M41">
-        <f>K39/M39</f>
+      <c r="O41">
+        <f>M39/O39</f>
         <v>1.1360265080016894</v>
       </c>
-      <c r="P41">
-        <f>N39/P39</f>
+      <c r="R41">
+        <f>P39/R39</f>
         <v>0.96489834325253931</v>
       </c>
-      <c r="Q41">
-        <f>O39/Q39</f>
+      <c r="S41">
+        <f>Q39/S39</f>
         <v>1.2230334731804484</v>
       </c>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F42" t="s">
-        <v>21</v>
-      </c>
-      <c r="K42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="H44">
-        <f>D39/H39</f>
+    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="H42" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="M42" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q42" s="38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="J44">
+        <f>F39/J39</f>
         <v>2.9223750801877575</v>
       </c>
-      <c r="I44">
-        <f>E39/I39</f>
+      <c r="K44">
+        <f>G39/K39</f>
         <v>3.5292397478594806</v>
       </c>
-      <c r="L44">
-        <f>D39/L39</f>
+      <c r="N44">
+        <f>F39/N39</f>
         <v>2.8847161021107603</v>
       </c>
-      <c r="M44">
-        <f>E39/M39</f>
+      <c r="O44">
+        <f>G39/O39</f>
         <v>3.6161460942025161</v>
       </c>
-      <c r="P44">
-        <f>D39/P39</f>
+      <c r="R44">
+        <f>F39/R39</f>
         <v>2.1972765449728815</v>
       </c>
-      <c r="Q44">
-        <f>E39/Q39</f>
+      <c r="S44">
+        <f>G39/S39</f>
         <v>3.613777564483668</v>
       </c>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="G45" t="s">
-        <v>22</v>
-      </c>
-      <c r="K45" t="s">
-        <v>22</v>
+    <row r="45" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="I45" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="M45" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q45" s="38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="J47">
+        <f>+D39/J39</f>
+        <v>250.73154992421013</v>
+      </c>
+      <c r="K47">
+        <f>+E39/K39</f>
+        <v>296.96033717459085</v>
+      </c>
+      <c r="N47">
+        <f>+D39/N39</f>
+        <v>247.50051568571646</v>
+      </c>
+      <c r="O47">
+        <f>+E39/O39</f>
+        <v>304.27288598295451</v>
+      </c>
+      <c r="R47">
+        <f>+D39/R39</f>
+        <v>188.52013811237671</v>
+      </c>
+      <c r="S47">
+        <f>+E39/S39</f>
+        <v>304.0735911109233</v>
+      </c>
+    </row>
+    <row r="48" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="I48" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="M48" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q48" s="38" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="F2:I2"/>
+  <mergeCells count="16">
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="H2:K2"/>
     <mergeCell ref="B5:B14"/>
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="B27:B36"/>
-    <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>